<commit_message>
Update-Add UnitPrice to Stock
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/MCStock.xlsx
+++ b/bin/Debug/Template/MCStock.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MachineDeptApp\MachineDeptApp v1.0.0.8\Source Code\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A05A315-8C6E-4824-BF0E-6AD3F42CBA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A04BD8-B320-4454-B9EC-AC2EA58D72EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="3495" windowWidth="20730" windowHeight="11040" xr2:uid="{52A4A616-E32B-479B-A2FD-84B20778D881}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{52A4A616-E32B-479B-A2FD-84B20778D881}"/>
   </bookViews>
   <sheets>
     <sheet name="RachhanSystem" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RachhanSystem!$A$5:$H$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RachhanSystem!$A$5:$K$6</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -24,12 +24,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Issue:</t>
     <phoneticPr fontId="0"/>
@@ -81,17 +92,41 @@
   </si>
   <si>
     <t>MC vs OBS</t>
+  </si>
+  <si>
+    <t>ប្រភេទ</t>
+  </si>
+  <si>
+    <t>RM Type</t>
+  </si>
+  <si>
+    <t>ទឹកប្រាក់</t>
+  </si>
+  <si>
+    <t>ទឹកប្រាក់សរុប</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>តម្លៃឯកតា</t>
+  </si>
+  <si>
+    <t>Amount OBS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;$&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +193,27 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Khmer OS Battambang"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Khmer OS Battambang"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
       <name val="Khmer OS Battambang"/>
     </font>
   </fonts>
@@ -218,7 +274,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -249,9 +305,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -266,13 +319,56 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="7"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -294,18 +390,6 @@
         <color rgb="FF00B050"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -320,9 +404,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -360,7 +444,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -466,7 +550,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -608,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,77 +704,96 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H1"/>
+      <selection pane="bottomLeft" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="10" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
-    <col min="3" max="5" width="21.85546875" style="12" customWidth="1"/>
-    <col min="6" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="19.42578125" style="11" customWidth="1"/>
+    <col min="8" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:11" ht="33.75" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
-    <row r="2" spans="1:8" ht="23.25" customHeight="1">
+    <row r="2" spans="1:11" ht="23.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="21.75" thickBot="1">
+    <row r="3" spans="1:11" ht="21.75" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:11" s="6" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -698,55 +801,77 @@
         <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="J5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:11" ht="21">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="20"/>
+    </row>
+    <row r="7" spans="1:11" ht="24.75" customHeight="1">
+      <c r="C7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:H5" xr:uid="{006D9A6D-0870-493B-8EA4-BD30CF2CA0AC}"/>
+  <autoFilter ref="A5:K6" xr:uid="{006D9A6D-0870-493B-8EA4-BD30CF2CA0AC}"/>
   <mergeCells count="2">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+  <conditionalFormatting sqref="I6">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.55118110236220474" header="0" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;P / &amp;N Page</oddFooter>
   </headerFooter>

</xml_diff>